<commit_message>
Changed "on display" to "small frames"
</commit_message>
<xml_diff>
--- a/Middle Assignment 1/TestDesignTechique1_PhamHongAnh.xlsx
+++ b/Middle Assignment 1/TestDesignTechique1_PhamHongAnh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FCE797-8C69-427A-B3BC-1A3EEC7F712D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE61453C-2991-4127-9913-C7F5FF0E9F56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,25 +556,10 @@
     <t>Verify that when the number behind the decimal point is 0.1, the number is rounded down to 0 as the nearest integer</t>
   </si>
   <si>
-    <t>Verify that if the number of photos in the photo list is between 1 and 5, the exact number of photos is displayed on the photo list</t>
-  </si>
-  <si>
     <t>Verify that the maximum number of photos in the photo list is 15</t>
   </si>
   <si>
-    <t>Verify that if the number of photos in the photo list is between 6 and 15, there are always 5 photos on display</t>
-  </si>
-  <si>
-    <t>Verify that the first photo from left to right of the 5 photos on display is displayed on the big frame</t>
-  </si>
-  <si>
     <t>Verify that if there is no photo in the photo list, the big frame will show the "NO IMAGE" message</t>
-  </si>
-  <si>
-    <t>Verify that the &gt; button can navigate users from the current photo on big frame to the next photo on the right</t>
-  </si>
-  <si>
-    <t>Verify that the &lt; button can navigate users from the current photo on big frame to the previous photo on the left</t>
   </si>
   <si>
     <t>Verify that when the last photo in the photo list is on big frame, the &gt; button is disabled and the &lt; button is still enabled</t>
@@ -587,6 +572,21 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that the number of photos in the photo list could be higher than 5 </t>
+  </si>
+  <si>
+    <t>Verify that if the number of photos in the photo list is between 1 and 5, the exact number of photos is displayed in the 5 small frames</t>
+  </si>
+  <si>
+    <t>Verify that if the number of photos in the photo list is between 6 and 15, there are always 5 photos in the 5 small frames</t>
+  </si>
+  <si>
+    <t>Verify that the first photo from left to right of the 5 photos in the 5 small frames is displayed on the big frame</t>
+  </si>
+  <si>
+    <t>Verify that the &lt; button can navigate users from the current photo on big frame to the previous photo on the left in the small frames</t>
+  </si>
+  <si>
+    <t>Verify that the &gt; button can navigate users from the current photo on big frame to the next photo on the right in the small frames</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1028,8 @@
   </sheetPr>
   <dimension ref="A1:Z1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1547,7 +1547,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -2235,7 +2235,7 @@
         <v>33</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -2322,12 +2322,12 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" spans="1:26" ht="35.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" ht="44.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>34</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="16"/>
@@ -2343,7 +2343,7 @@
         <v>35</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="16"/>
@@ -2359,7 +2359,7 @@
         <v>36</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="16"/>
@@ -2375,7 +2375,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="16"/>
@@ -2391,7 +2391,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -2407,7 +2407,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
         <v>40</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D47" s="12"/>
     </row>
@@ -2438,7 +2438,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -2454,7 +2454,7 @@
         <v>42</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -2470,7 +2470,7 @@
         <v>43</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>

</xml_diff>

<commit_message>
Reworded tc descrips + 1st draft steps and outputs
</commit_message>
<xml_diff>
--- a/Middle Assignment 1/TestDesignTechique1_PhamHongAnh.xlsx
+++ b/Middle Assignment 1/TestDesignTechique1_PhamHongAnh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E2A176-B7CB-45E9-B717-40737BE43217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AA120F-C09A-423B-94F2-15CFD79C8966}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,7 +620,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="115">
   <si>
     <t>ID</t>
   </si>
@@ -893,20 +893,7 @@
     <t>Check default - The first photo is on the big frame</t>
   </si>
   <si>
-    <t>Select a product with 1 or more photos</t>
-  </si>
-  <si>
-    <t>The first photo is on the big frame</t>
-  </si>
-  <si>
-    <t>1. Select a product
-2. Select a photo in the product's photo list</t>
-  </si>
-  <si>
     <t>The selected photo is on the big frame</t>
-  </si>
-  <si>
-    <t>Select a product with no photos</t>
   </si>
   <si>
     <t>The big frame shows a "NO IMAGE" text</t>
@@ -930,9 +917,6 @@
     <t xml:space="preserve">At the first photo, the &gt; button is enabled </t>
   </si>
   <si>
-    <t xml:space="preserve">Click on the &gt; button </t>
-  </si>
-  <si>
     <t>1. Users can click on the &gt; button
 2. Users can navigate to the next photos</t>
   </si>
@@ -941,37 +925,67 @@
 2. Users can navigate to the previous photos</t>
   </si>
   <si>
-    <t xml:space="preserve">Click on the &lt; button </t>
+    <t>Users cannot click on the &gt; button</t>
   </si>
   <si>
-    <t>1. Select the last photo 
-2. Click on the &gt; button</t>
+    <t>Users cannot click on the &lt; button</t>
   </si>
   <si>
-    <t>1. Select the first photo 
-2. Click on the &lt; button</t>
+    <t>1. Users can click on the &gt; button
+2. Users can navigate to next photos</t>
   </si>
   <si>
-    <t>1. Select the last photo 
-2. Click on the &lt; button</t>
+    <t xml:space="preserve">1. Select a product with 2 photos
+2. Click on the &gt; button </t>
   </si>
   <si>
-    <t>1. Select the first photo 
-2. Click on the &gt; button</t>
+    <t xml:space="preserve">1. Select a product with 2 photos
+2. Click on the second photo of the product
+3. Click on the &lt; button </t>
   </si>
   <si>
-    <t>Users cannot click the &gt; button</t>
+    <t xml:space="preserve">1. Select a product with 2 photos
+2. Click on the second photo of the product
+3. Click on the &gt; button </t>
   </si>
   <si>
-    <t>Users cannot click the &lt; button</t>
+    <t xml:space="preserve">1. Select a product with 2 photos
+2. Click on the first photo of the product
+3. Click on the &lt; button </t>
   </si>
   <si>
-    <t>1. Users can click the &lt; button
-2. Users can navigate to the previous photos</t>
+    <t xml:space="preserve">1. Select a product with 2 photos
+2. Click on the first photo of the product
+3. Click on the &gt; button </t>
   </si>
   <si>
-    <t>1. Users can click the &gt; button
-2. Users can navigate to next photos</t>
+    <t>When it is neither the first nor the last photo, both butttons &lt;&gt; are enabled</t>
+  </si>
+  <si>
+    <t>1. Select a product with 3 photos
+2. Click on the second photo 
+3. Click on the &gt; button
+4. Click on the second photo again
+5. Click on the &lt; button</t>
+  </si>
+  <si>
+    <t>1. When it is the second photo, users can click on the &gt; button to move to the third photo
+2. When it is the second photo, users can click on the &lt; button to move to the first photo</t>
+  </si>
+  <si>
+    <t>Select a product with no photo</t>
+  </si>
+  <si>
+    <t>1. Select a product with 1 photo
+2. Select a product with 2 photos</t>
+  </si>
+  <si>
+    <t>1. When there is 1 photo, the only photo is on the big frame
+2. When there is 2 photo, the first photo is on the big frame</t>
+  </si>
+  <si>
+    <t>1. Select a product with 2 photos
+2. Click on a photo in the product's photo list</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1167,11 +1181,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1210,34 +1261,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1250,6 +1275,41 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1471,16 +1531,16 @@
   </sheetPr>
   <dimension ref="A1:Z1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7265625" style="13" customWidth="1"/>
     <col min="2" max="2" width="37.7265625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="29.08984375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="36.453125" style="15" customWidth="1"/>
     <col min="5" max="9" width="12.6328125" style="10"/>
   </cols>
   <sheetData>
@@ -1531,17 +1591,17 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1561,17 +1621,17 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1960,17 +2020,17 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -2356,17 +2416,17 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="20"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="30"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -2392,10 +2452,10 @@
       <c r="B26" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="31" t="s">
         <v>70</v>
       </c>
       <c r="E26" s="3"/>
@@ -2432,9 +2492,7 @@
       <c r="C27" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="21" t="s">
-        <v>70</v>
-      </c>
+      <c r="D27" s="32"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="8"/>
@@ -2467,9 +2525,7 @@
       <c r="C28" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="21" t="s">
-        <v>70</v>
-      </c>
+      <c r="D28" s="32"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -2504,9 +2560,7 @@
       <c r="C29" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="21" t="s">
-        <v>70</v>
-      </c>
+      <c r="D29" s="33"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="8"/>
@@ -2529,17 +2583,17 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="20"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="30"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -2568,7 +2622,7 @@
       <c r="C31" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D31" s="31" t="s">
         <v>71</v>
       </c>
       <c r="E31" s="3"/>
@@ -2605,9 +2659,7 @@
       <c r="C32" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="21" t="s">
-        <v>71</v>
-      </c>
+      <c r="D32" s="32"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -2642,9 +2694,7 @@
       <c r="C33" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="21" t="s">
-        <v>71</v>
-      </c>
+      <c r="D33" s="33"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -2669,17 +2719,17 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -2699,17 +2749,17 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="26"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="23"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -2732,13 +2782,13 @@
       <c r="A36" s="7">
         <v>28</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="17" t="s">
         <v>84</v>
       </c>
       <c r="E36" s="3"/>
@@ -2755,10 +2805,10 @@
       <c r="B37" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="17" t="s">
         <v>85</v>
       </c>
       <c r="E37" s="3"/>
@@ -2772,13 +2822,13 @@
         <f t="shared" ca="1" si="2"/>
         <v>30</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="17" t="s">
         <v>86</v>
       </c>
       <c r="E38" s="3"/>
@@ -2792,13 +2842,13 @@
         <f t="shared" ca="1" si="2"/>
         <v>31</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="27" t="s">
+      <c r="D39" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E39" s="3"/>
@@ -2815,10 +2865,10 @@
       <c r="B40" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="27" t="s">
+      <c r="D40" s="17" t="s">
         <v>88</v>
       </c>
       <c r="E40" s="3"/>
@@ -2827,19 +2877,19 @@
       <c r="H40" s="3"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="50" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <f ca="1">IF(OFFSET(A41,-1,0) ="",OFFSET(A41,-2,0)+1,OFFSET(A41,-1,0)+1 )</f>
         <v>33</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>91</v>
+      <c r="C41" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -2855,11 +2905,11 @@
       <c r="B42" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>93</v>
+      <c r="C42" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -2875,53 +2925,53 @@
       <c r="B43" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>95</v>
+      <c r="C43" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="26"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="23"/>
     </row>
     <row r="45" spans="1:26" ht="62" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
-        <v>34</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="D45" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="19" t="s">
         <v>103</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="51.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <f t="shared" ref="A46:A50" ca="1" si="3">IF(OFFSET(A46,-1,0) ="",OFFSET(A46,-2,0)+1,OFFSET(A46,-1,0)+1 )</f>
-        <v>35</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="D46" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>104</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -2932,16 +2982,16 @@
     <row r="47" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" s="21" t="s">
-        <v>110</v>
+        <v>38</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -2952,16 +3002,16 @@
     <row r="48" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
-      </c>
-      <c r="B48" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="D48" s="21" t="s">
-        <v>112</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -2972,16 +3022,16 @@
     <row r="49" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>111</v>
+        <v>40</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -2992,16 +3042,16 @@
     <row r="50" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="21" t="s">
-        <v>113</v>
+        <v>41</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -3009,11 +3059,19 @@
       <c r="H50" s="3"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
+    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>42</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>110</v>
+      </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -13823,7 +13881,7 @@
       <c r="I1041"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="A44:I44"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A34:I34"/>
@@ -13832,6 +13890,8 @@
     <mergeCell ref="A35:I35"/>
     <mergeCell ref="A30:I30"/>
     <mergeCell ref="A25:I25"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D31:D33"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
"Close-to-last photo" case + No action in output
</commit_message>
<xml_diff>
--- a/Middle Assignment 1/TestDesignTechique1_PhamHongAnh.xlsx
+++ b/Middle Assignment 1/TestDesignTechique1_PhamHongAnh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C8E6E5-FAC3-4762-87F3-08EC6C274A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEC226A-ABA4-47F3-8272-793C04960C5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,6 +57,30 @@
           <t xml:space="preserve">
 Use action verbs e.g., check…
 Chỉ xét view</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{3555CCA9-B73F-4451-B455-CF960679FA22}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+output -&gt; user thấy kết quả thôi</t>
         </r>
       </text>
     </comment>
@@ -471,7 +495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B40" authorId="0" shapeId="0" xr:uid="{57D51019-7130-447B-9427-4BB1EA71A533}">
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{57D51019-7130-447B-9427-4BB1EA71A533}">
       <text>
         <r>
           <rPr>
@@ -495,7 +519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B41" authorId="0" shapeId="0" xr:uid="{E0698B9E-8FA2-4D4C-B3C0-97F77515A335}">
+    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{E0698B9E-8FA2-4D4C-B3C0-97F77515A335}">
       <text>
         <r>
           <rPr>
@@ -519,7 +543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{C3F2739D-3978-4237-8A8F-2362707F905E}">
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{C3F2739D-3978-4237-8A8F-2362707F905E}">
       <text>
         <r>
           <rPr>
@@ -543,7 +567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="0" shapeId="0" xr:uid="{B551684C-6F08-4266-BC1C-BF5D2B40754A}">
+    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{B551684C-6F08-4266-BC1C-BF5D2B40754A}">
       <text>
         <r>
           <rPr>
@@ -567,7 +591,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{CA952FCE-CB0F-448F-A285-D23103BA9902}">
+    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{477BE6E6-A86F-4A64-9A75-46DC8D1E51BC}">
       <text>
         <r>
           <rPr>
@@ -591,7 +615,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B51" authorId="0" shapeId="0" xr:uid="{3BDDA6C6-3425-4CC5-AD7A-8089D69DA596}">
+    <comment ref="E43" authorId="0" shapeId="0" xr:uid="{6EA896BB-4FC5-458C-B815-BBDD9F90BCBF}">
       <text>
         <r>
           <rPr>
@@ -611,7 +635,55 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-State transition - khi nhấn vào ảnh thứ 2 và 14 thì cả 2 nút &lt;&gt; vẫn enabled</t>
+Shorten + tách ra thành big frame và small frame</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B48" authorId="0" shapeId="0" xr:uid="{3BDDA6C6-3425-4CC5-AD7A-8089D69DA596}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tách thành 2 cases riêng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B49" authorId="0" shapeId="0" xr:uid="{3DD9FD98-08A7-4835-9D2A-AA550F35663D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tách thành 2 cases riêng</t>
         </r>
       </text>
     </comment>
@@ -620,7 +692,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="110">
   <si>
     <t>ID</t>
   </si>
@@ -781,12 +853,6 @@
     <t xml:space="preserve">Select the product with the discounted price of ₫999,999,999 </t>
   </si>
   <si>
-    <t>Select the product with the discounted price of ₫250,000.49</t>
-  </si>
-  <si>
-    <t>Select the product with the discounted price of ₫250,000.51</t>
-  </si>
-  <si>
     <t>Select the product with the discounted price of ₫250,000.5</t>
   </si>
   <si>
@@ -799,28 +865,16 @@
     <t>Check rounding function - if discount price is a float with format x.y when y&lt;5</t>
   </si>
   <si>
-    <t>Check rounding function - if discount price is a float with format x.y when y=51</t>
-  </si>
-  <si>
-    <t>Check rounding function - if discount price is a float with format x.y when y=99</t>
-  </si>
-  <si>
     <t>Check rounding function - if discount price is a float with format x.y when y=1</t>
   </si>
   <si>
     <t>Select the product with the discounted price of ₫250,000.1</t>
   </si>
   <si>
-    <t>Check rounding function - if discount price is a float with format x.y when y=49</t>
-  </si>
-  <si>
     <t>Select the product with the discounted price of ₫250,000.3</t>
   </si>
   <si>
     <t>Select the product with the discounted price of ₫250,000.6</t>
-  </si>
-  <si>
-    <t>Select the product with the discounted price of ₫250,000.99</t>
   </si>
   <si>
     <t>Rounding up</t>
@@ -853,13 +907,7 @@
     <t>Select a product with 5 photos</t>
   </si>
   <si>
-    <t>Select a product with 15 photos</t>
-  </si>
-  <si>
     <t>The number of photos in the photo list is more than 5</t>
-  </si>
-  <si>
-    <t>Select a product with 6 photos</t>
   </si>
   <si>
     <t>Select a product with 1 photo</t>
@@ -890,12 +938,6 @@
     <t>The big frame shows a "NO IMAGE" text</t>
   </si>
   <si>
-    <t>Users can click on the &gt; button to navigate to the next photos</t>
-  </si>
-  <si>
-    <t>Users can click on the &lt; button to navigate to the previous photos</t>
-  </si>
-  <si>
     <t xml:space="preserve">At the last photo, the &gt; button is disabled </t>
   </si>
   <si>
@@ -906,24 +948,6 @@
   </si>
   <si>
     <t xml:space="preserve">At the first photo, the &gt; button is enabled </t>
-  </si>
-  <si>
-    <t>1. Users can click on the &gt; button
-2. Users can navigate to the next photos</t>
-  </si>
-  <si>
-    <t>1. Users can click on the &lt; button
-2. Users can navigate to the previous photos</t>
-  </si>
-  <si>
-    <t>Users cannot click on the &gt; button</t>
-  </si>
-  <si>
-    <t>Users cannot click on the &lt; button</t>
-  </si>
-  <si>
-    <t>1. Users can click on the &gt; button
-2. Users can navigate to next photos</t>
   </si>
   <si>
     <t xml:space="preserve">1. Select a product with 2 photos
@@ -950,20 +974,6 @@
 3. Click on the &gt; button </t>
   </si>
   <si>
-    <t>When it is neither the first nor the last photo, both butttons &lt;&gt; are enabled</t>
-  </si>
-  <si>
-    <t>1. Select a product with 3 photos
-2. Click on the second photo 
-3. Click on the &gt; button
-4. Click on the second photo again
-5. Click on the &lt; button</t>
-  </si>
-  <si>
-    <t>1. When it is the second photo, users can click on the &gt; button to move to the third photo
-2. When it is the second photo, users can click on the &lt; button to move to the first photo</t>
-  </si>
-  <si>
     <t>Select a product with no photo</t>
   </si>
   <si>
@@ -986,6 +996,51 @@
   </si>
   <si>
     <t>When users click on a photo in the photo list</t>
+  </si>
+  <si>
+    <t>Check the &gt; button when users select the close-to-last photo</t>
+  </si>
+  <si>
+    <t>Check the &lt; button when users select the close-to-first photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Select a product with 3 photos
+2. Click on the second photo 
+</t>
+  </si>
+  <si>
+    <t>The &gt; button is enabled</t>
+  </si>
+  <si>
+    <t>The &lt; button is enabled</t>
+  </si>
+  <si>
+    <t>1. Select a product with 6 photos
+2. Click on the &gt; button</t>
+  </si>
+  <si>
+    <t>1. Select a product with 15 photos
+2. Click on the &gt; button until reaching the last photo</t>
+  </si>
+  <si>
+    <t>The &gt; button works</t>
+  </si>
+  <si>
+    <t>The &lt; button works</t>
+  </si>
+  <si>
+    <t>1. The &lt; button is clickable
+2. The &lt; button navigates users to the previous photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The &gt; button is not clickable</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The &lt; button is not clickable</t>
+  </si>
+  <si>
+    <t>1. The &gt; button is clickable
+2. The &gt; button navigates users to next photos</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1194,35 +1249,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1303,13 +1334,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1529,10 +1554,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1041"/>
+  <dimension ref="A1:Z1038"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1592,7 +1617,7 @@
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -1622,7 +1647,7 @@
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -2021,7 +2046,7 @@
     </row>
     <row r="14" spans="1:26" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -2087,7 +2112,7 @@
     </row>
     <row r="16" spans="1:26" ht="25" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
-        <f t="shared" ref="A16:A33" ca="1" si="1">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
+        <f t="shared" ref="A16:A30" ca="1" si="1">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
         <v>12</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -2417,7 +2442,7 @@
     </row>
     <row r="25" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
@@ -2450,13 +2475,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -2487,12 +2512,15 @@
         <v>22</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="32"/>
+        <v>53</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="31"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="8"/>
@@ -2514,23 +2542,18 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="28" spans="1:26" ht="25" x14ac:dyDescent="0.35">
-      <c r="A28" s="7">
-        <f t="shared" ca="1" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="8"/>
+    <row r="28" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="30"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -2551,16 +2574,19 @@
     </row>
     <row r="29" spans="1:26" ht="25" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
-        <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="33"/>
+      <c r="D29" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="31"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="8"/>
@@ -2582,18 +2608,25 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="30"/>
+    <row r="30" spans="1:26" ht="25" x14ac:dyDescent="0.35">
+      <c r="A30" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="8"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -2612,184 +2645,138 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
-    <row r="31" spans="1:26" ht="25" x14ac:dyDescent="0.35">
-      <c r="A31" s="7">
+    <row r="31" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+    </row>
+    <row r="32" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
         <v>25</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
-    </row>
-    <row r="32" spans="1:26" ht="25" x14ac:dyDescent="0.35">
-      <c r="A32" s="7">
-        <f t="shared" ca="1" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="32"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
-      <c r="X32" s="2"/>
-      <c r="Y32" s="2"/>
-      <c r="Z32" s="2"/>
-    </row>
-    <row r="33" spans="1:26" ht="25" x14ac:dyDescent="0.35">
-      <c r="A33" s="7">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="33"/>
+      <c r="B33" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>73</v>
+      </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
-      <c r="X33" s="2"/>
-      <c r="Y33" s="2"/>
-      <c r="Z33" s="2"/>
-    </row>
-    <row r="34" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="24" t="s">
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <f t="shared" ref="A34:A37" ca="1" si="2">IF(OFFSET(A34,-1,0) ="",OFFSET(A34,-2,0)+1,OFFSET(A34,-1,0)+1 )</f>
+        <v>26</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="B36" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-      <c r="Z34" s="1"/>
-    </row>
-    <row r="35" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-      <c r="U35" s="1"/>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
-      <c r="Y35" s="1"/>
-      <c r="Z35" s="1"/>
-    </row>
-    <row r="36" spans="1:26" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
-        <v>28</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>112</v>
-      </c>
       <c r="C36" s="16" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -2797,19 +2784,19 @@
       <c r="H36" s="3"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:26" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
-        <f t="shared" ref="A37:A40" ca="1" si="2">IF(OFFSET(A37,-1,0) ="",OFFSET(A37,-2,0)+1,OFFSET(A37,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>29</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -2817,19 +2804,19 @@
       <c r="H37" s="3"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="50" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">IF(OFFSET(A38,-1,0) ="",OFFSET(A38,-2,0)+1,OFFSET(A38,-1,0)+1 )</f>
         <v>30</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>83</v>
+        <v>91</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -2837,19 +2824,19 @@
       <c r="H38" s="3"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:26" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">IF(OFFSET(A39,-1,0) ="",OFFSET(A39,-2,0)+1,OFFSET(A39,-1,0)+1 )</f>
         <v>31</v>
       </c>
-      <c r="B39" s="16" t="s">
-        <v>78</v>
+      <c r="B39" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="C39" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>84</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -2857,121 +2844,121 @@
       <c r="H39" s="3"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:26" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">IF(OFFSET(A40,-1,0) ="",OFFSET(A40,-2,0)+1,OFFSET(A40,-1,0)+1 )</f>
         <v>32</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="23"/>
+    </row>
+    <row r="42" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>33</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="6"/>
-    </row>
-    <row r="41" spans="1:26" ht="50" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
-        <f ca="1">IF(OFFSET(A41,-1,0) ="",OFFSET(A41,-2,0)+1,OFFSET(A41,-1,0)+1 )</f>
-        <v>33</v>
-      </c>
-      <c r="B41" s="16" t="s">
+      <c r="D42" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="51.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <f t="shared" ref="A43:A49" ca="1" si="3">IF(OFFSET(A43,-1,0) ="",OFFSET(A43,-2,0)+1,OFFSET(A43,-1,0)+1 )</f>
+        <v>34</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="6"/>
-    </row>
-    <row r="42" spans="1:26" ht="38" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
-        <f ca="1">IF(OFFSET(A42,-1,0) ="",OFFSET(A42,-2,0)+1,OFFSET(A42,-1,0)+1 )</f>
-        <v>34</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D42" s="16" t="s">
+      <c r="D43" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E43" s="16"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <f t="shared" ca="1" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="6"/>
-    </row>
-    <row r="43" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
-        <f ca="1">IF(OFFSET(A43,-1,0) ="",OFFSET(A43,-2,0)+1,OFFSET(A43,-1,0)+1 )</f>
-        <v>35</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="18" t="s">
+      <c r="D44" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <f t="shared" ca="1" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <f t="shared" ca="1" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" s="16" t="s">
         <v>108</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="23"/>
-    </row>
-    <row r="45" spans="1:26" ht="62" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
-        <v>36</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:26" ht="51.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
-        <f t="shared" ref="A46:A50" ca="1" si="3">IF(OFFSET(A46,-1,0) ="",OFFSET(A46,-2,0)+1,OFFSET(A46,-1,0)+1 )</f>
-        <v>37</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>96</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -2979,19 +2966,19 @@
       <c r="H46" s="3"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <f t="shared" ca="1" si="3"/>
         <v>38</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>97</v>
+        <v>89</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -2999,19 +2986,19 @@
       <c r="H47" s="3"/>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <f t="shared" ca="1" si="3"/>
         <v>39</v>
       </c>
-      <c r="B48" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>101</v>
+      <c r="B48" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -3019,19 +3006,19 @@
       <c r="H48" s="3"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <f t="shared" ca="1" si="3"/>
         <v>40</v>
       </c>
-      <c r="B49" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>103</v>
+      <c r="B49" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -3039,46 +3026,29 @@
       <c r="H49" s="3"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
-        <f t="shared" ca="1" si="3"/>
-        <v>41</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>99</v>
-      </c>
+    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="6"/>
-    </row>
-    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
-        <v>42</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>107</v>
-      </c>
+      <c r="I50" s="8"/>
+    </row>
+    <row r="51" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="7"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="6"/>
-    </row>
-    <row r="52" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="I51" s="8"/>
+    </row>
+    <row r="52" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="7"/>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -3087,9 +3057,9 @@
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="6"/>
-    </row>
-    <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I52" s="8"/>
+    </row>
+    <row r="53" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="7"/>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -3100,38 +3070,14 @@
       <c r="H53" s="3"/>
       <c r="I53" s="8"/>
     </row>
-    <row r="54" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="7"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="8"/>
-    </row>
-    <row r="55" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="7"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="8"/>
-    </row>
-    <row r="56" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="7"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="8"/>
+    <row r="54" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="9"/>
+    </row>
+    <row r="55" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="9"/>
+    </row>
+    <row r="56" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="9"/>
     </row>
     <row r="57" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
@@ -3159,12 +3105,36 @@
     </row>
     <row r="65" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="9"/>
+      <c r="B65"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
     </row>
     <row r="66" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="9"/>
+      <c r="B66"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
     </row>
     <row r="67" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A67" s="9"/>
+      <c r="B67"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+      <c r="I67"/>
     </row>
     <row r="68" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A68" s="9"/>
@@ -13847,51 +13817,16 @@
       <c r="H1038"/>
       <c r="I1038"/>
     </row>
-    <row r="1039" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A1039" s="9"/>
-      <c r="B1039"/>
-      <c r="C1039" s="14"/>
-      <c r="D1039" s="14"/>
-      <c r="E1039"/>
-      <c r="F1039"/>
-      <c r="G1039"/>
-      <c r="H1039"/>
-      <c r="I1039"/>
-    </row>
-    <row r="1040" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A1040" s="9"/>
-      <c r="B1040"/>
-      <c r="C1040" s="14"/>
-      <c r="D1040" s="14"/>
-      <c r="E1040"/>
-      <c r="F1040"/>
-      <c r="G1040"/>
-      <c r="H1040"/>
-      <c r="I1040"/>
-    </row>
-    <row r="1041" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A1041" s="9"/>
-      <c r="B1041"/>
-      <c r="C1041" s="14"/>
-      <c r="D1041" s="14"/>
-      <c r="E1041"/>
-      <c r="F1041"/>
-      <c r="G1041"/>
-      <c r="H1041"/>
-      <c r="I1041"/>
-    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A44:I44"/>
+  <mergeCells count="8">
+    <mergeCell ref="A41:I41"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A31:I31"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A28:I28"/>
     <mergeCell ref="A25:I25"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D31:D33"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Spelling + Deleted y=0 case
</commit_message>
<xml_diff>
--- a/Middle Assignment 1/TestDesignTechique1_PhamHongAnh.xlsx
+++ b/Middle Assignment 1/TestDesignTechique1_PhamHongAnh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEC226A-ABA4-47F3-8272-793C04960C5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB1D740-9D84-45F7-A0CB-824B8A00E5EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,7 +495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{57D51019-7130-447B-9427-4BB1EA71A533}">
+    <comment ref="B36" authorId="0" shapeId="0" xr:uid="{57D51019-7130-447B-9427-4BB1EA71A533}">
       <text>
         <r>
           <rPr>
@@ -519,7 +519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{E0698B9E-8FA2-4D4C-B3C0-97F77515A335}">
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{E0698B9E-8FA2-4D4C-B3C0-97F77515A335}">
       <text>
         <r>
           <rPr>
@@ -543,7 +543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{C3F2739D-3978-4237-8A8F-2362707F905E}">
+    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{C3F2739D-3978-4237-8A8F-2362707F905E}">
       <text>
         <r>
           <rPr>
@@ -567,7 +567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{B551684C-6F08-4266-BC1C-BF5D2B40754A}">
+    <comment ref="B41" authorId="0" shapeId="0" xr:uid="{B551684C-6F08-4266-BC1C-BF5D2B40754A}">
       <text>
         <r>
           <rPr>
@@ -591,7 +591,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{477BE6E6-A86F-4A64-9A75-46DC8D1E51BC}">
+    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{477BE6E6-A86F-4A64-9A75-46DC8D1E51BC}">
       <text>
         <r>
           <rPr>
@@ -615,7 +615,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E43" authorId="0" shapeId="0" xr:uid="{6EA896BB-4FC5-458C-B815-BBDD9F90BCBF}">
+    <comment ref="E42" authorId="0" shapeId="0" xr:uid="{6EA896BB-4FC5-458C-B815-BBDD9F90BCBF}">
       <text>
         <r>
           <rPr>
@@ -639,7 +639,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B48" authorId="0" shapeId="0" xr:uid="{3BDDA6C6-3425-4CC5-AD7A-8089D69DA596}">
+    <comment ref="B47" authorId="0" shapeId="0" xr:uid="{3BDDA6C6-3425-4CC5-AD7A-8089D69DA596}">
       <text>
         <r>
           <rPr>
@@ -663,7 +663,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0" shapeId="0" xr:uid="{3DD9FD98-08A7-4835-9D2A-AA550F35663D}">
+    <comment ref="B48" authorId="0" shapeId="0" xr:uid="{3DD9FD98-08A7-4835-9D2A-AA550F35663D}">
       <text>
         <r>
           <rPr>
@@ -692,7 +692,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="109">
   <si>
     <t>ID</t>
   </si>
@@ -865,12 +865,6 @@
     <t>Check rounding function - if discount price is a float with format x.y when y&lt;5</t>
   </si>
   <si>
-    <t>Check rounding function - if discount price is a float with format x.y when y=1</t>
-  </si>
-  <si>
-    <t>Select the product with the discounted price of ₫250,000.1</t>
-  </si>
-  <si>
     <t>Select the product with the discounted price of ₫250,000.3</t>
   </si>
   <si>
@@ -1041,6 +1035,9 @@
   <si>
     <t>1. The &gt; button is clickable
 2. The &gt; button navigates users to next photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the price is ₫1,000 </t>
   </si>
 </sst>
 </file>
@@ -1307,6 +1304,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1332,9 +1332,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1554,10 +1551,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1038"/>
+  <dimension ref="A1:Z1037"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1616,17 +1613,17 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
+      <c r="A2" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1646,17 +1643,17 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
+      <c r="A3" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -2045,17 +2042,17 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
+      <c r="A14" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -2112,7 +2109,7 @@
     </row>
     <row r="16" spans="1:26" ht="25" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
-        <f t="shared" ref="A16:A30" ca="1" si="1">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
+        <f t="shared" ref="A16:A27" ca="1" si="1">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
         <v>12</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -2227,7 +2224,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>48</v>
@@ -2441,17 +2438,17 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="30"/>
+      <c r="A25" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="31"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -2478,10 +2475,10 @@
         <v>54</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>61</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -2517,10 +2514,10 @@
       <c r="C27" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="31"/>
+      <c r="D27" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="21"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="8"/>
@@ -2543,17 +2540,17 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="30"/>
+      <c r="A28" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="31"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -2580,12 +2577,12 @@
         <v>56</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="31"/>
+        <v>57</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="21"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -2608,55 +2605,48 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30" spans="1:26" ht="25" x14ac:dyDescent="0.35">
-      <c r="A30" s="7">
-        <f t="shared" ca="1" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
-      <c r="X30" s="2"/>
-      <c r="Y30" s="2"/>
-      <c r="Z30" s="2"/>
+    <row r="30" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
+      <c r="A31" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="24"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -2675,48 +2665,38 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
+    <row r="32" spans="1:26" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>24</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
+        <f t="shared" ref="A33:A36" ca="1" si="2">IF(OFFSET(A33,-1,0) ="",OFFSET(A33,-2,0)+1,OFFSET(A33,-1,0)+1 )</f>
         <v>25</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>94</v>
+      <c r="B33" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="C33" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="17" t="s">
         <v>72</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>73</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -2724,19 +2704,19 @@
       <c r="H33" s="3"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
-        <f t="shared" ref="A34:A37" ca="1" si="2">IF(OFFSET(A34,-1,0) ="",OFFSET(A34,-2,0)+1,OFFSET(A34,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>26</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>13</v>
+      <c r="B34" s="16" t="s">
+        <v>93</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -2744,19 +2724,19 @@
       <c r="H34" s="3"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <f t="shared" ca="1" si="2"/>
         <v>27</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -2764,19 +2744,19 @@
       <c r="H35" s="3"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <f t="shared" ca="1" si="2"/>
         <v>28</v>
       </c>
-      <c r="B36" s="16" t="s">
-        <v>71</v>
+      <c r="B36" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -2784,19 +2764,19 @@
       <c r="H36" s="3"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="50" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">IF(OFFSET(A37,-1,0) ="",OFFSET(A37,-2,0)+1,OFFSET(A37,-1,0)+1 )</f>
         <v>29</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>12</v>
+      <c r="B37" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>77</v>
+        <v>89</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -2804,19 +2784,19 @@
       <c r="H37" s="3"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" ht="50" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <f ca="1">IF(OFFSET(A38,-1,0) ="",OFFSET(A38,-2,0)+1,OFFSET(A38,-1,0)+1 )</f>
         <v>30</v>
       </c>
-      <c r="B38" s="16" t="s">
-        <v>78</v>
+      <c r="B38" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>91</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -2824,83 +2804,83 @@
       <c r="H38" s="3"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <f ca="1">IF(OFFSET(A39,-1,0) ="",OFFSET(A39,-2,0)+1,OFFSET(A39,-1,0)+1 )</f>
         <v>31</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D39" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="24"/>
+    </row>
+    <row r="41" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>32</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="51.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <f t="shared" ref="A42:A48" ca="1" si="3">IF(OFFSET(A42,-1,0) ="",OFFSET(A42,-2,0)+1,OFFSET(A42,-1,0)+1 )</f>
+        <v>33</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="16"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <f t="shared" ca="1" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="B43" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="6"/>
-    </row>
-    <row r="40" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7">
-        <f ca="1">IF(OFFSET(A40,-1,0) ="",OFFSET(A40,-2,0)+1,OFFSET(A40,-1,0)+1 )</f>
-        <v>32</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="23"/>
-    </row>
-    <row r="42" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
-        <v>33</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C42" s="19" t="s">
+      <c r="C43" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D42" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="51.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
-        <f t="shared" ref="A43:A49" ca="1" si="3">IF(OFFSET(A43,-1,0) ="",OFFSET(A43,-2,0)+1,OFFSET(A43,-1,0)+1 )</f>
-        <v>34</v>
-      </c>
-      <c r="B43" s="16" t="s">
+      <c r="D43" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="E43" s="16"/>
+      <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -2912,13 +2892,13 @@
         <v>35</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>107</v>
+        <v>84</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -2932,12 +2912,12 @@
         <v>36</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="16" t="s">
         <v>106</v>
       </c>
       <c r="E45" s="3"/>
@@ -2946,19 +2926,19 @@
       <c r="H45" s="3"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <f t="shared" ca="1" si="3"/>
         <v>37</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>108</v>
+        <v>87</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -2966,19 +2946,19 @@
       <c r="H46" s="3"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <f t="shared" ca="1" si="3"/>
         <v>38</v>
       </c>
-      <c r="B47" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>109</v>
+      <c r="B47" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -2992,13 +2972,13 @@
         <v>39</v>
       </c>
       <c r="B48" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="D48" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>100</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -3006,27 +2986,18 @@
       <c r="H48" s="3"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
-        <f t="shared" ca="1" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>101</v>
-      </c>
+    <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="6"/>
-    </row>
-    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I49" s="8"/>
+    </row>
+    <row r="50" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="7"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -3059,16 +3030,8 @@
       <c r="H52" s="3"/>
       <c r="I52" s="8"/>
     </row>
-    <row r="53" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="7"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="8"/>
+    <row r="53" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="9"/>
     </row>
     <row r="54" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -3102,6 +3065,14 @@
     </row>
     <row r="64" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="9"/>
+      <c r="B64"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="I64"/>
     </row>
     <row r="65" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="9"/>
@@ -13806,25 +13777,14 @@
       <c r="H1037"/>
       <c r="I1037"/>
     </row>
-    <row r="1038" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A1038" s="9"/>
-      <c r="B1038"/>
-      <c r="C1038" s="14"/>
-      <c r="D1038" s="14"/>
-      <c r="E1038"/>
-      <c r="F1038"/>
-      <c r="G1038"/>
-      <c r="H1038"/>
-      <c r="I1038"/>
-    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="A40:I40"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A30:I30"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A31:I31"/>
     <mergeCell ref="A28:I28"/>
     <mergeCell ref="A25:I25"/>
   </mergeCells>

</xml_diff>

<commit_message>
updated y=0 case? :+1:
</commit_message>
<xml_diff>
--- a/Middle Assignment 1/TestDesignTechique1_PhamHongAnh.xlsx
+++ b/Middle Assignment 1/TestDesignTechique1_PhamHongAnh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB1D740-9D84-45F7-A0CB-824B8A00E5EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67291098-4CA2-4395-97D7-86BE8F5BD1A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,7 +495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B36" authorId="0" shapeId="0" xr:uid="{57D51019-7130-447B-9427-4BB1EA71A533}">
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{57D51019-7130-447B-9427-4BB1EA71A533}">
       <text>
         <r>
           <rPr>
@@ -519,7 +519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{E0698B9E-8FA2-4D4C-B3C0-97F77515A335}">
+    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{E0698B9E-8FA2-4D4C-B3C0-97F77515A335}">
       <text>
         <r>
           <rPr>
@@ -543,7 +543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{C3F2739D-3978-4237-8A8F-2362707F905E}">
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{C3F2739D-3978-4237-8A8F-2362707F905E}">
       <text>
         <r>
           <rPr>
@@ -567,7 +567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B41" authorId="0" shapeId="0" xr:uid="{B551684C-6F08-4266-BC1C-BF5D2B40754A}">
+    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{B551684C-6F08-4266-BC1C-BF5D2B40754A}">
       <text>
         <r>
           <rPr>
@@ -591,7 +591,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{477BE6E6-A86F-4A64-9A75-46DC8D1E51BC}">
+    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{477BE6E6-A86F-4A64-9A75-46DC8D1E51BC}">
       <text>
         <r>
           <rPr>
@@ -615,7 +615,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E42" authorId="0" shapeId="0" xr:uid="{6EA896BB-4FC5-458C-B815-BBDD9F90BCBF}">
+    <comment ref="E43" authorId="0" shapeId="0" xr:uid="{6EA896BB-4FC5-458C-B815-BBDD9F90BCBF}">
       <text>
         <r>
           <rPr>
@@ -639,7 +639,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0" shapeId="0" xr:uid="{3BDDA6C6-3425-4CC5-AD7A-8089D69DA596}">
+    <comment ref="B48" authorId="0" shapeId="0" xr:uid="{3BDDA6C6-3425-4CC5-AD7A-8089D69DA596}">
       <text>
         <r>
           <rPr>
@@ -663,7 +663,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B48" authorId="0" shapeId="0" xr:uid="{3DD9FD98-08A7-4835-9D2A-AA550F35663D}">
+    <comment ref="B49" authorId="0" shapeId="0" xr:uid="{3DD9FD98-08A7-4835-9D2A-AA550F35663D}">
       <text>
         <r>
           <rPr>
@@ -692,7 +692,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -1039,6 +1039,12 @@
   <si>
     <t xml:space="preserve">When the price is ₫1,000 </t>
   </si>
+  <si>
+    <t>Check rounding function - if discount price is a float with format x.y when y=0</t>
+  </si>
+  <si>
+    <t>Select the product with the discounted price of ₫250,000.0</t>
+  </si>
 </sst>
 </file>
 
@@ -1173,7 +1179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1246,11 +1252,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1331,6 +1346,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1551,10 +1578,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1037"/>
+  <dimension ref="A1:Z1038"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2570,7 +2597,7 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" spans="1:26" ht="25" x14ac:dyDescent="0.35">
-      <c r="A29" s="7">
+      <c r="A29" s="32">
         <v>23</v>
       </c>
       <c r="B29" s="11" t="s">
@@ -2582,11 +2609,11 @@
       <c r="D29" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="21"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="8"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="35"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -2605,48 +2632,55 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="25" t="s">
+    <row r="30" spans="1:26" ht="25" x14ac:dyDescent="0.35">
+      <c r="A30" s="7">
+        <f t="shared" ref="A30" ca="1" si="2">IF(OFFSET(A30,-1,0) ="",OFFSET(A30,-2,0)+1,OFFSET(A30,-1,0)+1 )</f>
+        <v>24</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+    </row>
+    <row r="31" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-    </row>
-    <row r="31" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="24"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -2665,38 +2699,48 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" spans="1:26" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
-        <v>24</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="6"/>
+    <row r="32" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
-        <f t="shared" ref="A33:A36" ca="1" si="2">IF(OFFSET(A33,-1,0) ="",OFFSET(A33,-2,0)+1,OFFSET(A33,-1,0)+1 )</f>
         <v>25</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>13</v>
+      <c r="B33" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -2704,19 +2748,19 @@
       <c r="H33" s="3"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="A34:A37" ca="1" si="3">IF(OFFSET(A34,-1,0) ="",OFFSET(A34,-2,0)+1,OFFSET(A34,-1,0)+1 )</f>
         <v>26</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>93</v>
+      <c r="B34" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -2724,19 +2768,19 @@
       <c r="H34" s="3"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>27</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -2744,19 +2788,19 @@
       <c r="H35" s="3"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>28</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>12</v>
+      <c r="B36" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -2764,19 +2808,19 @@
       <c r="H36" s="3"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" ht="50" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
-        <f ca="1">IF(OFFSET(A37,-1,0) ="",OFFSET(A37,-2,0)+1,OFFSET(A37,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="3"/>
         <v>29</v>
       </c>
-      <c r="B37" s="16" t="s">
-        <v>76</v>
+      <c r="B37" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>90</v>
+        <v>101</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -2784,19 +2828,19 @@
       <c r="H37" s="3"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="50" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <f ca="1">IF(OFFSET(A38,-1,0) ="",OFFSET(A38,-2,0)+1,OFFSET(A38,-1,0)+1 )</f>
         <v>30</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>94</v>
+      <c r="B38" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -2804,83 +2848,83 @@
       <c r="H38" s="3"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <f ca="1">IF(OFFSET(A39,-1,0) ="",OFFSET(A39,-2,0)+1,OFFSET(A39,-1,0)+1 )</f>
         <v>31</v>
       </c>
       <c r="B39" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <f ca="1">IF(OFFSET(A40,-1,0) ="",OFFSET(A40,-2,0)+1,OFFSET(A40,-1,0)+1 )</f>
+        <v>32</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C40" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D40" s="19" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+    <row r="41" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="24"/>
-    </row>
-    <row r="41" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="24"/>
+    </row>
+    <row r="42" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>32</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B42" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C42" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D42" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="51.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
-        <f t="shared" ref="A42:A48" ca="1" si="3">IF(OFFSET(A42,-1,0) ="",OFFSET(A42,-2,0)+1,OFFSET(A42,-1,0)+1 )</f>
+    <row r="43" spans="1:9" ht="51.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <f t="shared" ref="A43:A49" ca="1" si="4">IF(OFFSET(A43,-1,0) ="",OFFSET(A43,-2,0)+1,OFFSET(A43,-1,0)+1 )</f>
         <v>33</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B43" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C43" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D43" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="E42" s="16"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="6"/>
-    </row>
-    <row r="43" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
-        <f t="shared" ca="1" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E43" s="3"/>
+      <c r="E43" s="16"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -2888,17 +2932,17 @@
     </row>
     <row r="44" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
-        <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>34</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>104</v>
+        <v>85</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>105</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -2908,17 +2952,17 @@
     </row>
     <row r="45" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
-        <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>35</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>106</v>
+        <v>84</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -2926,19 +2970,19 @@
       <c r="H45" s="3"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
-        <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>36</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>107</v>
+        <v>86</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>106</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -2946,19 +2990,19 @@
       <c r="H46" s="3"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <f t="shared" ca="1" si="3"/>
-        <v>38</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>98</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -2968,17 +3012,17 @@
     </row>
     <row r="48" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
-        <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>38</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>97</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -2986,18 +3030,27 @@
       <c r="H48" s="3"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="7"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
+    <row r="49" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <f t="shared" ca="1" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="8"/>
-    </row>
-    <row r="50" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="7"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -3030,8 +3083,16 @@
       <c r="H52" s="3"/>
       <c r="I52" s="8"/>
     </row>
-    <row r="53" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
+    <row r="53" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="7"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="8"/>
     </row>
     <row r="54" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -3065,14 +3126,6 @@
     </row>
     <row r="64" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="9"/>
-      <c r="B64"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64"/>
-      <c r="F64"/>
-      <c r="G64"/>
-      <c r="H64"/>
-      <c r="I64"/>
     </row>
     <row r="65" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="9"/>
@@ -13777,14 +13830,25 @@
       <c r="H1037"/>
       <c r="I1037"/>
     </row>
+    <row r="1038" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1038" s="9"/>
+      <c r="B1038"/>
+      <c r="C1038" s="14"/>
+      <c r="D1038" s="14"/>
+      <c r="E1038"/>
+      <c r="F1038"/>
+      <c r="G1038"/>
+      <c r="H1038"/>
+      <c r="I1038"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A41:I41"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:I31"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A32:I32"/>
     <mergeCell ref="A28:I28"/>
     <mergeCell ref="A25:I25"/>
   </mergeCells>

</xml_diff>